<commit_message>
small upd + pthw
</commit_message>
<xml_diff>
--- a/Raspisanie_1_gruppa.xlsx
+++ b/Raspisanie_1_gruppa.xlsx
@@ -5,11 +5,11 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gleb/Desktop/Projects/tinkoff/trash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gleb/Desktop/Projects/tinkoff/Auto homework/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16020" yWindow="0" windowWidth="12780" windowHeight="18000"/>
+    <workbookView xWindow="18760" yWindow="0" windowWidth="10040" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>Время</t>
   </si>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.6640625" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -847,9 +847,7 @@
       <c r="F10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="G10" s="7"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>